<commit_message>
reduced some codes on cases sensitives
</commit_message>
<xml_diff>
--- a/Week01_report.xlsx
+++ b/Week01_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="62">
   <si>
     <t>Student ID</t>
   </si>
@@ -184,13 +184,10 @@
     <t>Week01</t>
   </si>
   <si>
-    <t>Git_task.png, Index_file_creation.png, create_Html_file_on_Name.png, dulingo_update.png</t>
-  </si>
-  <si>
-    <t>Index_file_creation.png, dulingo_update.png</t>
-  </si>
-  <si>
-    <t>Git_task.png, Index_file_creation.png, dulingo_update.png</t>
+    <t>Git_Task, Index_File_Updation, create_Html_file_on_Name, dulingo_update</t>
+  </si>
+  <si>
+    <t>dulingo_update</t>
   </si>
   <si>
     <t>Completed</t>
@@ -202,7 +199,7 @@
     <t>Week: Week01</t>
   </si>
   <si>
-    <t>Generated: 2023-09-02 09:47:23 AM</t>
+    <t>Generated: 2023-09-02 11:47:58 AM</t>
   </si>
 </sst>
 </file>
@@ -582,7 +579,7 @@
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="89.7109375" customWidth="1"/>
+    <col min="4" max="4" width="73.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -614,7 +611,7 @@
         <v>55</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -631,7 +628,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -645,7 +642,7 @@
         <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -659,7 +656,7 @@
         <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -676,7 +673,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -693,7 +690,7 @@
         <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -710,24 +707,21 @@
         <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>55</v>
       </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>60</v>
+      <c r="E9" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -741,7 +735,7 @@
         <v>55</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -758,7 +752,7 @@
         <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -772,7 +766,7 @@
         <v>55</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -786,7 +780,7 @@
         <v>55</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -803,7 +797,7 @@
         <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -820,7 +814,7 @@
         <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -837,7 +831,7 @@
         <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -854,7 +848,7 @@
         <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -871,7 +865,7 @@
         <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -888,7 +882,7 @@
         <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -905,7 +899,7 @@
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -919,7 +913,7 @@
         <v>55</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -933,7 +927,7 @@
         <v>55</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -950,7 +944,7 @@
         <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -967,7 +961,7 @@
         <v>56</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -984,34 +978,31 @@
         <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C26" t="s">
         <v>55</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E26" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
json file removed and enhansed code with default task
</commit_message>
<xml_diff>
--- a/Week01_report.xlsx
+++ b/Week01_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
   <si>
     <t>Student ID</t>
   </si>
@@ -73,6 +73,9 @@
     <t>PPP014</t>
   </si>
   <si>
+    <t>PPP015</t>
+  </si>
+  <si>
     <t>PPP016</t>
   </si>
   <si>
@@ -148,6 +151,9 @@
     <t>Naveen Bromiyo A R</t>
   </si>
   <si>
+    <t>Kalai Selvi</t>
+  </si>
+  <si>
     <t>Madhan Karthick</t>
   </si>
   <si>
@@ -199,7 +205,7 @@
     <t>Week: Week01</t>
   </si>
   <si>
-    <t>Generated: 2023-09-02 11:58:20 AM</t>
+    <t>Generated: 2023-09-02 12:23:24 PM</t>
   </si>
 </sst>
 </file>
@@ -570,7 +576,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -605,13 +611,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -619,16 +625,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -636,13 +642,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -650,13 +656,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -664,16 +670,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -681,16 +687,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -698,16 +704,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -715,13 +721,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -729,13 +735,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -743,16 +749,16 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -760,13 +766,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -774,13 +780,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -788,16 +794,16 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -805,16 +811,16 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -822,16 +828,16 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -839,16 +845,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -856,16 +862,16 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -873,16 +879,16 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -890,30 +896,33 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>49</v>
+      <c r="B21" t="s">
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -921,30 +930,27 @@
         <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s">
-        <v>51</v>
+      <c r="B23" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -952,16 +958,16 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -969,40 +975,57 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>54</v>
+      <c r="B26" t="s">
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated task pngs for week1
</commit_message>
<xml_diff>
--- a/Week01_report.xlsx
+++ b/Week01_report.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SwathipriyaSundaram\Student report\StudentsReport\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EED0FD-4FA7-4738-8B2F-C71BA7B9D247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
   <si>
     <t>Student ID</t>
   </si>
@@ -214,8 +220,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,13 +297,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -335,7 +349,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -369,6 +383,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -403,9 +418,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -578,12 +594,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
@@ -593,7 +611,7 @@
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -630,7 +648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -650,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -667,7 +685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -684,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -701,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -721,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -741,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -758,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -775,7 +793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -792,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -809,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -826,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -846,7 +864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -863,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -883,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -903,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -923,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -943,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -963,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -983,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1000,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1017,27 +1035,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C24" t="s">
         <v>58</v>
       </c>
-      <c r="D24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" t="s">
-        <v>62</v>
+      <c r="E24" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1054,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1074,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1091,12 +1106,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>64</v>
       </c>

</xml_diff>